<commit_message>
chore: Update UI styles and fix import in Login.py
</commit_message>
<xml_diff>
--- a/doc/data.xlsx
+++ b/doc/data.xlsx
@@ -20,7 +20,7 @@
     <sheet name="云璃展示" sheetId="9" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IOS畅销榜!$A$1:$Q$85</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IOS畅销榜!$A$1:$Q$87</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">云璃展示!$A$1:$E$509</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -676,7 +676,7 @@
     <t>2024/8/14-2024/9/4</t>
   </si>
   <si>
-    <t>美16德9法10英22日1韩1港8台1</t>
+    <t>美16德28法29英22日1韩1港8台3</t>
   </si>
   <si>
     <t>鸣潮折枝</t>
@@ -11083,12 +11083,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:S91"/>
+  <dimension ref="A1:S104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="I89" sqref="I89"/>
+      <selection pane="topRight" activeCell="G90" sqref="G90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -14224,8 +14224,281 @@
       <c r="R91" s="2"/>
       <c r="S91" s="2"/>
     </row>
+    <row r="92" spans="1:19">
+      <c r="A92" s="2"/>
+      <c r="B92" s="34"/>
+      <c r="C92" s="2"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="2"/>
+      <c r="G92" s="2"/>
+      <c r="H92" s="2"/>
+      <c r="I92" s="33"/>
+      <c r="J92" s="2"/>
+      <c r="K92" s="2"/>
+      <c r="L92" s="2"/>
+      <c r="M92" s="2"/>
+      <c r="N92" s="2"/>
+      <c r="O92" s="2"/>
+      <c r="P92" s="2"/>
+      <c r="Q92" s="2"/>
+      <c r="R92" s="2"/>
+      <c r="S92" s="2"/>
+    </row>
+    <row r="93" spans="1:19">
+      <c r="A93" s="2"/>
+      <c r="B93" s="34"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="2"/>
+      <c r="H93" s="2"/>
+      <c r="I93" s="33"/>
+      <c r="J93" s="2"/>
+      <c r="K93" s="2"/>
+      <c r="L93" s="2"/>
+      <c r="M93" s="2"/>
+      <c r="N93" s="2"/>
+      <c r="O93" s="2"/>
+      <c r="P93" s="2"/>
+      <c r="Q93" s="2"/>
+      <c r="R93" s="2"/>
+      <c r="S93" s="2"/>
+    </row>
+    <row r="94" spans="1:19">
+      <c r="A94" s="2"/>
+      <c r="B94" s="34"/>
+      <c r="C94" s="2"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+      <c r="G94" s="2"/>
+      <c r="H94" s="2"/>
+      <c r="I94" s="33"/>
+      <c r="J94" s="2"/>
+      <c r="K94" s="2"/>
+      <c r="L94" s="2"/>
+      <c r="M94" s="2"/>
+      <c r="N94" s="2"/>
+      <c r="O94" s="2"/>
+      <c r="P94" s="2"/>
+      <c r="Q94" s="2"/>
+      <c r="R94" s="2"/>
+      <c r="S94" s="2"/>
+    </row>
+    <row r="95" spans="1:19">
+      <c r="A95" s="2"/>
+      <c r="B95" s="34"/>
+      <c r="C95" s="2"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+      <c r="G95" s="2"/>
+      <c r="H95" s="2"/>
+      <c r="I95" s="33"/>
+      <c r="J95" s="2"/>
+      <c r="K95" s="2"/>
+      <c r="L95" s="2"/>
+      <c r="M95" s="2"/>
+      <c r="N95" s="2"/>
+      <c r="O95" s="2"/>
+      <c r="P95" s="2"/>
+      <c r="Q95" s="2"/>
+      <c r="R95" s="2"/>
+      <c r="S95" s="2"/>
+    </row>
+    <row r="96" spans="1:19">
+      <c r="A96" s="2"/>
+      <c r="B96" s="34"/>
+      <c r="C96" s="2"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+      <c r="G96" s="2"/>
+      <c r="H96" s="2"/>
+      <c r="I96" s="33"/>
+      <c r="J96" s="2"/>
+      <c r="K96" s="2"/>
+      <c r="L96" s="2"/>
+      <c r="M96" s="2"/>
+      <c r="N96" s="2"/>
+      <c r="O96" s="2"/>
+      <c r="P96" s="2"/>
+      <c r="Q96" s="2"/>
+      <c r="R96" s="2"/>
+      <c r="S96" s="2"/>
+    </row>
+    <row r="97" spans="1:19">
+      <c r="A97" s="2"/>
+      <c r="B97" s="34"/>
+      <c r="C97" s="2"/>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+      <c r="G97" s="2"/>
+      <c r="H97" s="2"/>
+      <c r="I97" s="33"/>
+      <c r="J97" s="2"/>
+      <c r="K97" s="2"/>
+      <c r="L97" s="2"/>
+      <c r="M97" s="2"/>
+      <c r="N97" s="2"/>
+      <c r="O97" s="2"/>
+      <c r="P97" s="2"/>
+      <c r="Q97" s="2"/>
+      <c r="R97" s="2"/>
+      <c r="S97" s="2"/>
+    </row>
+    <row r="98" spans="1:19">
+      <c r="A98" s="2"/>
+      <c r="B98" s="34"/>
+      <c r="C98" s="2"/>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+      <c r="G98" s="2"/>
+      <c r="H98" s="2"/>
+      <c r="I98" s="33"/>
+      <c r="J98" s="2"/>
+      <c r="K98" s="2"/>
+      <c r="L98" s="2"/>
+      <c r="M98" s="2"/>
+      <c r="N98" s="2"/>
+      <c r="O98" s="2"/>
+      <c r="P98" s="2"/>
+      <c r="Q98" s="2"/>
+      <c r="R98" s="2"/>
+      <c r="S98" s="2"/>
+    </row>
+    <row r="99" spans="1:19">
+      <c r="A99" s="2"/>
+      <c r="B99" s="34"/>
+      <c r="C99" s="2"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="2"/>
+      <c r="G99" s="2"/>
+      <c r="H99" s="2"/>
+      <c r="I99" s="33"/>
+      <c r="J99" s="2"/>
+      <c r="K99" s="2"/>
+      <c r="L99" s="2"/>
+      <c r="M99" s="2"/>
+      <c r="N99" s="2"/>
+      <c r="O99" s="2"/>
+      <c r="P99" s="2"/>
+      <c r="Q99" s="2"/>
+      <c r="R99" s="2"/>
+      <c r="S99" s="2"/>
+    </row>
+    <row r="100" spans="1:19">
+      <c r="A100" s="2"/>
+      <c r="B100" s="34"/>
+      <c r="C100" s="2"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
+      <c r="G100" s="2"/>
+      <c r="H100" s="2"/>
+      <c r="I100" s="33"/>
+      <c r="J100" s="2"/>
+      <c r="K100" s="2"/>
+      <c r="L100" s="2"/>
+      <c r="M100" s="2"/>
+      <c r="N100" s="2"/>
+      <c r="O100" s="2"/>
+      <c r="P100" s="2"/>
+      <c r="Q100" s="2"/>
+      <c r="R100" s="2"/>
+      <c r="S100" s="2"/>
+    </row>
+    <row r="101" spans="1:19">
+      <c r="A101" s="2"/>
+      <c r="B101" s="34"/>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+      <c r="H101" s="2"/>
+      <c r="I101" s="33"/>
+      <c r="J101" s="2"/>
+      <c r="K101" s="2"/>
+      <c r="L101" s="2"/>
+      <c r="M101" s="2"/>
+      <c r="N101" s="2"/>
+      <c r="O101" s="2"/>
+      <c r="P101" s="2"/>
+      <c r="Q101" s="2"/>
+      <c r="R101" s="2"/>
+      <c r="S101" s="2"/>
+    </row>
+    <row r="102" spans="1:19">
+      <c r="A102" s="2"/>
+      <c r="B102" s="34"/>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+      <c r="G102" s="2"/>
+      <c r="H102" s="2"/>
+      <c r="I102" s="33"/>
+      <c r="J102" s="2"/>
+      <c r="K102" s="2"/>
+      <c r="L102" s="2"/>
+      <c r="M102" s="2"/>
+      <c r="N102" s="2"/>
+      <c r="O102" s="2"/>
+      <c r="P102" s="2"/>
+      <c r="Q102" s="2"/>
+      <c r="R102" s="2"/>
+      <c r="S102" s="2"/>
+    </row>
+    <row r="103" spans="1:19">
+      <c r="A103" s="2"/>
+      <c r="B103" s="34"/>
+      <c r="C103" s="2"/>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
+      <c r="H103" s="2"/>
+      <c r="I103" s="33"/>
+      <c r="J103" s="2"/>
+      <c r="K103" s="2"/>
+      <c r="L103" s="2"/>
+      <c r="M103" s="2"/>
+      <c r="N103" s="2"/>
+      <c r="O103" s="2"/>
+      <c r="P103" s="2"/>
+      <c r="Q103" s="2"/>
+      <c r="R103" s="2"/>
+      <c r="S103" s="2"/>
+    </row>
+    <row r="104" spans="1:19">
+      <c r="A104" s="2"/>
+      <c r="B104" s="34"/>
+      <c r="C104" s="2"/>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
+      <c r="F104" s="2"/>
+      <c r="G104" s="2"/>
+      <c r="H104" s="2"/>
+      <c r="I104" s="33"/>
+      <c r="J104" s="2"/>
+      <c r="K104" s="2"/>
+      <c r="L104" s="2"/>
+      <c r="M104" s="2"/>
+      <c r="N104" s="2"/>
+      <c r="O104" s="2"/>
+      <c r="P104" s="2"/>
+      <c r="Q104" s="2"/>
+      <c r="R104" s="2"/>
+      <c r="S104" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:Q85">
+  <autoFilter ref="A1:Q87">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>